<commit_message>
admin register user data parsley, student dang ki nhom
</commit_message>
<xml_diff>
--- a/Danh_sach_de_tai.xlsx
+++ b/Danh_sach_de_tai.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="9">
   <si>
     <t>STT</t>
   </si>
@@ -35,52 +35,13 @@
     <t>Điểm</t>
   </si>
   <si>
-    <t>Nguyá»…n VÄƒn PhÃ¡c</t>
-  </si>
-  <si>
-    <t>PhÃ¢n tÃ­ch, thiáº¿t káº¿ há»‡ thá»‘ng thÃ´ng tin cho cÃ¡c dá»± Ã¡n pháº§n má»m</t>
-  </si>
-  <si>
-    <t>PhÃ¢n tÃ­ch, thiáº¿t káº¿ pháº§n má»m X9</t>
-  </si>
-  <si>
-    <t>PhÃ¢n tÃ­ch thiáº¿t káº¿ pháº§n má»m X1</t>
-  </si>
-  <si>
-    <t>Kháº£o sÃ¡t, phÃ¢n tÃ­ch, thiáº¿t káº¿ website</t>
-  </si>
-  <si>
-    <t>PhÃ¢n tÃ­ch thiáº¿t káº¿ website bÃ¡n hÃ ng</t>
-  </si>
-  <si>
-    <t>PhÃ¢n tÃ­ch, thiáº¿t káº¿ pháº§n má»m X2</t>
-  </si>
-  <si>
-    <t>PhÃ¢n tÃ­ch, thiáº¿t káº¿ pháº§n má»m X3</t>
-  </si>
-  <si>
-    <t>PhÃ¢n tÃ­ch, thiáº¿t káº¿ pháº§n má»m X4</t>
-  </si>
-  <si>
-    <t>PhÃ¢n tÃ­ch, thiáº¿t káº¿ pháº§n má»m X5</t>
-  </si>
-  <si>
-    <t>PhÃ¢n tÃ­ch, thiáº¿t káº¿ pháº§n má»m X6</t>
-  </si>
-  <si>
-    <t>PhÃ¢n tÃ­ch, thiáº¿t káº¿ pháº§n má»m X7</t>
-  </si>
-  <si>
-    <t>PhÃ¢n tÃ­ch, thiáº¿t káº¿ pháº§n má»m X8</t>
-  </si>
-  <si>
-    <t>ThÃ¡i Thá»‹ Thanh VÃ¢n</t>
-  </si>
-  <si>
-    <t>láº­p trÃ¬nh web</t>
-  </si>
-  <si>
-    <t>PhÃ¢n tÃ­ch thiáº¿t káº¿ xÃ¢y dá»±ng web Ä‘Äƒng kÃ½ thá»±c táº­p cÆ¡ sá»Ÿ chuyÃªn ngÃ nh</t>
+    <t>Nguyễn Văn Phác</t>
+  </si>
+  <si>
+    <t>Phân tích, thiết kế hệ thống thông tin cho các dự án phần mềm</t>
+  </si>
+  <si>
+    <t>Phân tích, thiết kế phần mềm X9</t>
   </si>
 </sst>
 </file>
@@ -419,7 +380,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:F14"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
@@ -464,222 +425,6 @@
         <v>8</v>
       </c>
       <c r="F2"/>
-    </row>
-    <row r="3" spans="1:6">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3">
-        <v>3</v>
-      </c>
-      <c r="D3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E3" t="s">
-        <v>9</v>
-      </c>
-      <c r="F3"/>
-    </row>
-    <row r="4" spans="1:6">
-      <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C4">
-        <v>2</v>
-      </c>
-      <c r="D4" t="s">
-        <v>10</v>
-      </c>
-      <c r="E4" t="s">
-        <v>11</v>
-      </c>
-      <c r="F4"/>
-    </row>
-    <row r="5" spans="1:6">
-      <c r="A5">
-        <v>4</v>
-      </c>
-      <c r="B5" t="s">
-        <v>6</v>
-      </c>
-      <c r="C5">
-        <v>4</v>
-      </c>
-      <c r="D5" t="s">
-        <v>7</v>
-      </c>
-      <c r="E5" t="s">
-        <v>12</v>
-      </c>
-      <c r="F5"/>
-    </row>
-    <row r="6" spans="1:6">
-      <c r="A6">
-        <v>5</v>
-      </c>
-      <c r="B6" t="s">
-        <v>6</v>
-      </c>
-      <c r="C6">
-        <v>5</v>
-      </c>
-      <c r="D6" t="s">
-        <v>7</v>
-      </c>
-      <c r="E6" t="s">
-        <v>13</v>
-      </c>
-      <c r="F6"/>
-    </row>
-    <row r="7" spans="1:6">
-      <c r="A7">
-        <v>6</v>
-      </c>
-      <c r="B7" t="s">
-        <v>6</v>
-      </c>
-      <c r="C7">
-        <v>6</v>
-      </c>
-      <c r="D7" t="s">
-        <v>7</v>
-      </c>
-      <c r="E7" t="s">
-        <v>13</v>
-      </c>
-      <c r="F7"/>
-    </row>
-    <row r="8" spans="1:6">
-      <c r="A8">
-        <v>7</v>
-      </c>
-      <c r="B8" t="s">
-        <v>6</v>
-      </c>
-      <c r="C8">
-        <v>7</v>
-      </c>
-      <c r="D8" t="s">
-        <v>7</v>
-      </c>
-      <c r="E8" t="s">
-        <v>14</v>
-      </c>
-      <c r="F8"/>
-    </row>
-    <row r="9" spans="1:6">
-      <c r="A9">
-        <v>8</v>
-      </c>
-      <c r="B9" t="s">
-        <v>6</v>
-      </c>
-      <c r="C9">
-        <v>8</v>
-      </c>
-      <c r="D9" t="s">
-        <v>7</v>
-      </c>
-      <c r="E9" t="s">
-        <v>13</v>
-      </c>
-      <c r="F9"/>
-    </row>
-    <row r="10" spans="1:6">
-      <c r="A10">
-        <v>9</v>
-      </c>
-      <c r="B10" t="s">
-        <v>6</v>
-      </c>
-      <c r="C10">
-        <v>9</v>
-      </c>
-      <c r="D10" t="s">
-        <v>7</v>
-      </c>
-      <c r="E10" t="s">
-        <v>15</v>
-      </c>
-      <c r="F10"/>
-    </row>
-    <row r="11" spans="1:6">
-      <c r="A11">
-        <v>10</v>
-      </c>
-      <c r="B11" t="s">
-        <v>6</v>
-      </c>
-      <c r="C11">
-        <v>10</v>
-      </c>
-      <c r="D11" t="s">
-        <v>7</v>
-      </c>
-      <c r="E11" t="s">
-        <v>16</v>
-      </c>
-      <c r="F11"/>
-    </row>
-    <row r="12" spans="1:6">
-      <c r="A12">
-        <v>11</v>
-      </c>
-      <c r="B12" t="s">
-        <v>6</v>
-      </c>
-      <c r="C12">
-        <v>11</v>
-      </c>
-      <c r="D12" t="s">
-        <v>7</v>
-      </c>
-      <c r="E12" t="s">
-        <v>17</v>
-      </c>
-      <c r="F12"/>
-    </row>
-    <row r="13" spans="1:6">
-      <c r="A13">
-        <v>12</v>
-      </c>
-      <c r="B13" t="s">
-        <v>6</v>
-      </c>
-      <c r="C13">
-        <v>12</v>
-      </c>
-      <c r="D13" t="s">
-        <v>7</v>
-      </c>
-      <c r="E13" t="s">
-        <v>18</v>
-      </c>
-      <c r="F13"/>
-    </row>
-    <row r="14" spans="1:6">
-      <c r="A14">
-        <v>13</v>
-      </c>
-      <c r="B14" t="s">
-        <v>19</v>
-      </c>
-      <c r="C14">
-        <v>14</v>
-      </c>
-      <c r="D14" t="s">
-        <v>20</v>
-      </c>
-      <c r="E14" t="s">
-        <v>21</v>
-      </c>
-      <c r="F14"/>
     </row>
   </sheetData>
   <sheetProtection sheet="false" objects="false" scenarios="false" formatCells="false" formatColumns="false" formatRows="false" insertColumns="false" insertRows="false" insertHyperlinks="false" deleteColumns="false" deleteRows="false" selectLockedCells="false" sort="false" autoFilter="false" pivotTables="false" selectUnlockedCells="false"/>

</xml_diff>

<commit_message>
sua sidebar, hoan thien chuc nang
</commit_message>
<xml_diff>
--- a/Danh_sach_de_tai.xlsx
+++ b/Danh_sach_de_tai.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="10">
   <si>
     <t>STT</t>
   </si>
@@ -26,22 +26,25 @@
     <t>Nhóm</t>
   </si>
   <si>
-    <t>Định hướng</t>
-  </si>
-  <si>
     <t>Đề tài</t>
   </si>
   <si>
     <t>Điểm</t>
   </si>
   <si>
-    <t>gv1</t>
-  </si>
-  <si>
-    <t>Phân tích, thiết kế hệ thống thông tin cho các dự án phần mềm</t>
-  </si>
-  <si>
-    <t>Phân tích, thiết kế phần mềm X9</t>
+    <t>giaovien1</t>
+  </si>
+  <si>
+    <t>detai1</t>
+  </si>
+  <si>
+    <t>detai1nhom2</t>
+  </si>
+  <si>
+    <t>giaovien2</t>
+  </si>
+  <si>
+    <t>nothin</t>
   </si>
 </sst>
 </file>
@@ -380,7 +383,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
@@ -388,7 +391,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:5">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -404,27 +407,51 @@
       <c r="E1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
-        <v>5</v>
-      </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:5">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C2">
         <v>1</v>
       </c>
       <c r="D2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2"/>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3">
+        <v>2</v>
+      </c>
+      <c r="D3" t="s">
         <v>7</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E3"/>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
         <v>8</v>
       </c>
-      <c r="F2"/>
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E4"/>
     </row>
   </sheetData>
   <sheetProtection sheet="false" objects="false" scenarios="false" formatCells="false" formatColumns="false" formatRows="false" insertColumns="false" insertRows="false" insertHyperlinks="false" deleteColumns="false" deleteRows="false" selectLockedCells="false" sort="false" autoFilter="false" pivotTables="false" selectUnlockedCells="false"/>

</xml_diff>